<commit_message>
version 2.0 (add new feat/redis+queue/change_logger)
</commit_message>
<xml_diff>
--- a/infrastructure/folders/buffer/write_sample/sample.xlsx
+++ b/infrastructure/folders/buffer/write_sample/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\aclhemy_pr\src\infrastructure\buffer\write_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\robot_presale\src\infrastructure\folders\buffer\write_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFC3969-58AA-455A-A7F6-D84EDAB470F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BC7E7E-138A-4FF7-8993-CB299A7D4BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Расчет" sheetId="1" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>НОМЕР СТРОКИ ИЗ АРХИВА</t>
   </si>
   <si>
-    <t>№ ПОСЛЕДНЕГО ЗАПРОСА ИЗ АРХИВА</t>
-  </si>
-  <si>
     <t>ГДЕ НАШЛИ</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>$, СТОИМОСТЬ ЗАКУПКИ ЗИП</t>
+  </si>
+  <si>
+    <t>ШАССИ</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -421,36 +421,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -492,8 +468,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -829,8 +803,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -843,12 +817,12 @@
     <col min="6" max="6" width="13.21875" style="8" customWidth="1"/>
     <col min="7" max="7" width="18" style="8" customWidth="1"/>
     <col min="8" max="9" width="9.21875" style="26" customWidth="1"/>
-    <col min="10" max="13" width="9.21875" style="8" customWidth="1"/>
-    <col min="14" max="14" width="9.21875" style="26" customWidth="1"/>
-    <col min="15" max="18" width="9.21875" style="8" customWidth="1"/>
-    <col min="19" max="22" width="9.21875" style="26" customWidth="1"/>
-    <col min="23" max="24" width="9.21875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="12.109375" style="8" customWidth="1"/>
+    <col min="10" max="14" width="9.21875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" style="26" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" style="8" hidden="1" customWidth="1"/>
+    <col min="17" max="19" width="9.21875" style="8" customWidth="1"/>
+    <col min="20" max="23" width="9.21875" style="26" customWidth="1"/>
+    <col min="24" max="25" width="9.21875" style="8" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="10.33203125" style="8" customWidth="1"/>
     <col min="27" max="27" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="9.21875" style="8"/>
@@ -876,65 +850,65 @@
       <c r="G1" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="34" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Z1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="AA1" s="32" t="s">
         <v>60</v>
-      </c>
-      <c r="AA1" s="34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -954,34 +928,34 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21"/>
-      <c r="N2" s="27" t="str">
-        <f>IF(T2="","",T2*2+S2)</f>
-        <v/>
-      </c>
-      <c r="O2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="27" t="str">
+        <f>IF(U2="","",U2*2+T2)</f>
+        <v/>
+      </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
-      <c r="R2" s="35" t="str">
+      <c r="R2" s="21"/>
+      <c r="S2" s="33" t="str">
         <f>IF(E2="","",E2*G2)</f>
         <v/>
       </c>
-      <c r="S2" s="27" t="str">
-        <f t="shared" ref="S2" si="0">IF(T2="","",T2/2)</f>
-        <v/>
-      </c>
-      <c r="T2" s="22"/>
-      <c r="U2" s="27" t="str">
-        <f t="shared" ref="U2" si="1">IF(T2="","",(T2*2+S2)*1.15)</f>
-        <v/>
-      </c>
+      <c r="T2" s="27" t="str">
+        <f t="shared" ref="T2" si="0">IF(U2="","",U2/2)</f>
+        <v/>
+      </c>
+      <c r="U2" s="22"/>
       <c r="V2" s="27" t="str">
-        <f>IF(U2="","",N2*E2*0.1)</f>
-        <v/>
-      </c>
-      <c r="W2" s="21"/>
+        <f t="shared" ref="V2" si="1">IF(U2="","",(U2*2+T2)*1.15)</f>
+        <v/>
+      </c>
+      <c r="W2" s="27" t="str">
+        <f>IF(V2="","",O2*E2*0.1)</f>
+        <v/>
+      </c>
       <c r="X2" s="21"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="33"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="31"/>
       <c r="AA2" s="20"/>
     </row>
   </sheetData>
@@ -1033,7 +1007,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="23" t="e">
-        <f>SUM(Расчет!V:V)*B1*B2</f>
+        <f>SUM(Расчет!W:W)*B1*B2</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1042,7 +1016,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="23" t="e">
-        <f>SUM(Расчет!U:U)*B2*B1</f>
+        <f>SUM(Расчет!V:V)*B2*B1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1060,7 +1034,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <f>SUMIF(Расчет!M:M,"Нет результатов.",Расчет!E:E)</f>
+        <f>SUMIF(Расчет!N:N,"Нет результатов.",Расчет!E:E)</f>
         <v>0</v>
       </c>
     </row>
@@ -1077,7 +1051,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="15">
-        <f>SUMIF(Расчет!A:A,"*",Расчет!I:I)+SUMIFS(Расчет!U:U,Расчет!A:A,"*",Расчет!J:J,"")/1.15</f>
+        <f>SUMIF(Расчет!A:A,"*",Расчет!I:I)+SUMIFS(Расчет!V:V,Расчет!A:A,"*",Расчет!J:J,"")/1.15</f>
         <v>0</v>
       </c>
       <c r="C10" s="24">
@@ -1103,7 +1077,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="15">
-        <f>SUMIF(Расчет!A:A,"*",Расчет!R:R)</f>
+        <f>SUMIF(Расчет!A:A,"*",Расчет!S:S)</f>
         <v>0</v>
       </c>
       <c r="C12" s="24">
@@ -1158,8 +1132,8 @@
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:X3944"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,6 +1142,8 @@
     <col min="11" max="12" width="9.21875" style="15" customWidth="1"/>
     <col min="13" max="13" width="9.21875" customWidth="1"/>
     <col min="17" max="18" width="9.21875" style="15"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
@@ -1283,11 +1259,11 @@
         <v/>
       </c>
       <c r="N2" s="21" t="str">
-        <f>IF(Расчет!K2="","",Расчет!K2)</f>
+        <f>IF(Расчет!L2="","",Расчет!L2)</f>
         <v/>
       </c>
       <c r="O2" s="21" t="str">
-        <f>IF(Расчет!L2="","",Расчет!L2)</f>
+        <f>IF(Расчет!M2="","",Расчет!M2)</f>
         <v/>
       </c>
       <c r="P2" s="21" t="e">
@@ -1297,23 +1273,23 @@
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
       <c r="S2" s="21" t="str">
+        <f>IF(Расчет!P2="","",Расчет!P2)</f>
+        <v/>
+      </c>
+      <c r="T2" s="21" t="str">
+        <f>IF(Расчет!X2="","",Расчет!X2)</f>
+        <v/>
+      </c>
+      <c r="U2" s="21" t="str">
         <f>IF(Расчет!Y2="","",Расчет!Y2)</f>
         <v/>
       </c>
-      <c r="T2" s="21" t="str">
-        <f>IF(Расчет!W2="","",Расчет!W2)</f>
-        <v/>
-      </c>
-      <c r="U2" s="21" t="str">
-        <f>IF(Расчет!X2="","",Расчет!X2)</f>
-        <v/>
-      </c>
       <c r="V2" s="21" t="str">
-        <f>IF(Расчет!R2="","",Расчет!R2)</f>
+        <f>IF(Расчет!S2="","",Расчет!S2)</f>
         <v/>
       </c>
       <c r="W2" s="21" t="str">
-        <f>IF(Расчет!P2="",IF(Расчет!Z2="","",Расчет!Z2),Расчет!P2)</f>
+        <f>IF(Расчет!Q2="",IF(Расчет!Z2="","",Расчет!Z2),Расчет!Q2)</f>
         <v/>
       </c>
       <c r="X2" s="16"/>

</xml_diff>

<commit_message>
feat/search for categories in the archive
</commit_message>
<xml_diff>
--- a/infrastructure/folders/buffer/write_sample/sample.xlsx
+++ b/infrastructure/folders/buffer/write_sample/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\robot_presale\src\infrastructure\folders\buffer\write_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BC7E7E-138A-4FF7-8993-CB299A7D4BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEA9401-D51D-44CA-AD34-2DD550EFC3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Расчет" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>Прогноз Трудозатрат</t>
   </si>
   <si>
-    <t>Закупка</t>
-  </si>
-  <si>
     <t>№ запроса</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>ШАССИ</t>
+  </si>
+  <si>
+    <t>Категория</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -830,40 +830,40 @@
   <sheetData>
     <row r="1" spans="1:27" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>6</v>
@@ -875,40 +875,40 @@
         <v>8</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="V1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="X1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="AA1" s="32" t="s">
         <v>59</v>
-      </c>
-      <c r="AA1" s="32" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -1095,12 +1095,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="24">
@@ -1114,7 +1114,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="15">
         <f>(C10+(C11+C12)*3)*2</f>
@@ -1132,8 +1132,8 @@
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:X3944"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,10 +1214,10 @@
         <v>35</v>
       </c>
       <c r="W1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>